<commit_message>
tests generated SFHSA AGAIN
</commit_message>
<xml_diff>
--- a/results/final/analysis.xlsx
+++ b/results/final/analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GGPC\Documents\inverted-pendulum\results\final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99C75CC8-DF48-4600-9B5F-47C6C465BE77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{866A65FA-7DD0-4A16-8E97-045A6B2F113F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2D37EE88-7CE5-453F-8A1E-8027593ADD57}"/>
+    <workbookView xWindow="32676" yWindow="-6852" windowWidth="20256" windowHeight="10656" activeTab="1" xr2:uid="{2D37EE88-7CE5-453F-8A1E-8027593ADD57}"/>
   </bookViews>
   <sheets>
     <sheet name="ssm_performance" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -149,7 +149,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0E+00"/>
+    <numFmt numFmtId="164" formatCode="0.0E+00"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -183,7 +183,7 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -630,7 +630,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -2861,7 +2861,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84BAD1D1-374B-4CAE-BB18-F6D94CD51BA2}">
   <dimension ref="A1:H97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
@@ -5408,7 +5408,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87E9C886-9E82-4085-964F-204E546BA944}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>